<commit_message>
20 trials per block
</commit_message>
<xml_diff>
--- a/blocks.xlsx
+++ b/blocks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard Naar\Documents\dok\TARU\EEGManyLabs\Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Richard Naar\Documents\dok\TARU\EEGManyLabs\Task\spotlight_replication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB1A42E-018D-4F2C-B034-158142F64889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D430436B-2458-48F9-9143-D9738A113FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1230" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="7">
   <si>
     <t>attendCond</t>
   </si>
@@ -81,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -409,7 +410,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4">
@@ -450,6 +451,160 @@
       </c>
       <c r="C7">
         <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>